<commit_message>
2025-08-15 - Cambio de la clase a tienda - Cambio del nombre del metodo para leer el inventario a leer_inventario - Adición de un metodo para vender productos sin crear el codigo - Correción del metodo para leer el inventario - Creación de un borrador del codigo para vender un producto
</commit_message>
<xml_diff>
--- a/Inventario_1.xlsx
+++ b/Inventario_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,26 +453,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Splash Victoria Secret</t>
+          <t>Esencia</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>unidades</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Splash Pink</t>
+          <t>Bolsa de Regalo</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -483,118 +483,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Crema Corporal Valsy</t>
+          <t>Splash Pink</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Esencia</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>650</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Loción Possession</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>45</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Loción Expression</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>38</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Loción Lotus</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>14</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Bolsa de Regalo</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>15</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Bolsa de Regalo</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>15</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Bolsa de Regalo</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr">
         <is>
           <t>unidades</t>
         </is>

</xml_diff>

<commit_message>
2025-09-23 -> Se creo un menu para interactuar con la aplicacion -> Se corrigieron errores por la creación de inventarios -> Pendiente completar el menú para ventas -> Pendiente Agregar actualización de inventario
</commit_message>
<xml_diff>
--- a/Inventario_1.xlsx
+++ b/Inventario_1.xlsx
@@ -4,53 +4,27 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventario" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ventas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="precios" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD"/>
-  </numFmts>
-  <fonts count="6">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <charset val="1"/>
-      <family val="0"/>
-      <b val="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -64,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,57 +51,21 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -200,41 +138,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -242,218 +180,324 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Producto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Unidad</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Splash Pink</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Splash</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>unidades</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="3">
-      <c r="A3" s="5" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Esencia</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>450</v>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="B3" t="n">
+        <v>300</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>gramos</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="3">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Bolsa de Regalo</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Crema</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>unidades</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -463,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,80 +515,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Producto</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>Cantidad</t>
-        </is>
-      </c>
-      <c r="D1" s="6" t="inlineStr">
-        <is>
-          <t>Unidad</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="n">
-        <v>45918.77046770833</v>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>Bolsa de Regalo</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>45918</v>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>Splash Pink</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>unidades</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Esencia</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>300</v>
+      </c>
+      <c r="C3" t="n">
+        <v>600</v>
+      </c>
+      <c r="D3" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="n">
-        <v>45918</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Esencia</t>
-        </is>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Crema</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7000</v>
       </c>
       <c r="C4" t="n">
-        <v>60</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>gramos</t>
-        </is>
+        <v>14000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>